<commit_message>
Test bench en C et déplacement de la documentation
</commit_message>
<xml_diff>
--- a/compilateur/debug.xlsx
+++ b/compilateur/debug.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dossier principal\Documents\Phelma\Miniprojet_RISC_V\compilateur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gael\Documents\Phelma\Miniprojet_RISC_V\compilateur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AA3BA4C-4DB2-41C3-B615-ABBFFD461F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FFEE14-37E0-42D4-A14E-34C7957A0EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EAC9A174-8B8D-448D-B2C1-A8A055AA9D2D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{EAC9A174-8B8D-448D-B2C1-A8A055AA9D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>33222222222211111111110000000000</t>
   </si>
@@ -42,27 +42,12 @@
     <t>00000000000000000000000110110111</t>
   </si>
   <si>
-    <t>11111110010000010010000000000011</t>
-  </si>
-  <si>
-    <t>11111110110000011010000000000011</t>
-  </si>
-  <si>
     <t>00000000000000000000000000000000</t>
   </si>
   <si>
     <t>00000000000100011000000110010011</t>
   </si>
   <si>
-    <t>11111110100000011010000000000011</t>
-  </si>
-  <si>
-    <t>11111110100000010010000000000011</t>
-  </si>
-  <si>
-    <t>00000001110000110010000000000011</t>
-  </si>
-  <si>
     <t>00000010000000010000000100010011</t>
   </si>
   <si>
@@ -135,24 +120,6 @@
     <t>000000100000 00010 000 00110 0010011</t>
   </si>
   <si>
-    <t>0000000 00010 00110 010 11100 0100011</t>
-  </si>
-  <si>
-    <t>00000000001000110010111000100011</t>
-  </si>
-  <si>
-    <t>01111110011000011010001000100011</t>
-  </si>
-  <si>
-    <t>01111110011000011010011000100011</t>
-  </si>
-  <si>
-    <t>01111110011000000010010000100011</t>
-  </si>
-  <si>
-    <t>01111110011000011010010000100011</t>
-  </si>
-  <si>
     <t>00000100001100010000000001100011</t>
   </si>
   <si>
@@ -181,6 +148,45 @@
   </si>
   <si>
     <t>1111100100000001000000001 1100111</t>
+  </si>
+  <si>
+    <t>00000000011000010010111000100011</t>
+  </si>
+  <si>
+    <t>01111110001100110010001000100011</t>
+  </si>
+  <si>
+    <t>01111110001100110010011000100011</t>
+  </si>
+  <si>
+    <t>11111110010000110010000100000011</t>
+  </si>
+  <si>
+    <t>11111110110000110010000110000011</t>
+  </si>
+  <si>
+    <t>01111110000000110010010000100011</t>
+  </si>
+  <si>
+    <t>11111110100000110010000110000011</t>
+  </si>
+  <si>
+    <t>01111110001100110010010000100011</t>
+  </si>
+  <si>
+    <t>11111110100000110010000100000011</t>
+  </si>
+  <si>
+    <t>00000001110000010010001100000011</t>
+  </si>
+  <si>
+    <t>0000000 00110 00010 010 11100 0100011</t>
+  </si>
+  <si>
+    <t>111111100100 00110 010 00010 0000011</t>
+  </si>
+  <si>
+    <t>111111100000 00010 000 00010 0010011</t>
   </si>
 </sst>
 </file>
@@ -549,108 +555,114 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="26" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="2.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -659,23 +671,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -684,12 +696,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -698,12 +710,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F15">
         <v>5</v>
@@ -712,34 +724,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F18">
         <v>5</v>
@@ -784,12 +796,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -834,23 +846,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -892,93 +904,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="16" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="16" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>